<commit_message>
Bug fixes, initial setup of login screen
Refactor error handling and app initialization logic

Improved error handling in `LoginViewModel` by introducing a
`HasError` property, simplifying the logic for error visibility
in `LoginPage.xaml`. Removed the `StringNotNullOrEmptyConverter`
and updated bindings accordingly.

Modified `App.xaml.cs` to remove `MainPage` initialization in
the constructor, potentially enabling more dynamic navigation.

Updated `PVA-TruthOrDrink.xlsx` (binary file) with unspecified
changes.
</commit_message>
<xml_diff>
--- a/Docs/PVA-TruthOrDrink.xlsx
+++ b/Docs/PVA-TruthOrDrink.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bartl\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bartl\Source\Repos\TruthOrDrinkApp\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA0CF89-10E8-412E-B807-53C751A89445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8CAAF5-FF92-4EAB-AF20-1A278CF07A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -321,6 +321,32 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -348,32 +374,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -388,13 +388,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C7982798-4570-4176-9C2C-443621B1D38F}" name="Table3" displayName="Table3" ref="A1:E39" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C7982798-4570-4176-9C2C-443621B1D38F}" name="Table3" displayName="Table3" ref="A1:E39" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3">
   <autoFilter ref="A1:E39" xr:uid="{C7982798-4570-4176-9C2C-443621B1D38F}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DE80C90A-24F9-4708-9F78-1D58AAE0EE41}" name="Week"/>
-    <tableColumn id="2" xr3:uid="{ECE1A02A-F54E-4B6F-AFCC-73C4B85E81E4}" name="Focus / Theme" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{D1C1DD61-397C-4B71-94D7-716F14234F3A}" name="Task" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{9C784095-F8AC-4446-82CC-2A06497D389E}" name="Deliverable / Milestone" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{ECE1A02A-F54E-4B6F-AFCC-73C4B85E81E4}" name="Focus / Theme" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{D1C1DD61-397C-4B71-94D7-716F14234F3A}" name="Task" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{9C784095-F8AC-4446-82CC-2A06497D389E}" name="Deliverable / Milestone" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{6F0E62E7-BE0D-4D43-80E6-E2687A24653D}" name="Done (✓ when finished)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -689,8 +689,8 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +701,7 @@
     <col min="5" max="5" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -775,7 +775,7 @@
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>

</xml_diff>